<commit_message>
Added Store Endpoint for testing
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ltimindtree-my.sharepoint.com/personal/anik_10827551_ltimindtree_com/Documents/Desktop/pet_api_testing/pet_api_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="13_ncr:1_{FBE78F29-6822-4D92-A068-ECF30B48FA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19EC7731-3071-49EB-A233-02B296A3A6EB}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="13_ncr:1_{FBE78F29-6822-4D92-A068-ECF30B48FA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AF66A3F-9E33-423A-BA28-F0AC29841424}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="PostPet" sheetId="4" r:id="rId3"/>
     <sheet name="Status" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Store" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="26" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="287">
   <si>
     <t>id</t>
   </si>
@@ -798,14 +799,103 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>petID</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>shipDate</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>2025-05-14T09:56:59.041877</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>2025-04-23T09:56:59.041897</t>
+  </si>
+  <si>
+    <t>delivered</t>
+  </si>
+  <si>
+    <t>2025-04-18T09:56:59.041906</t>
+  </si>
+  <si>
+    <t>2025-04-20T09:56:59.041914</t>
+  </si>
+  <si>
+    <t>placed</t>
+  </si>
+  <si>
+    <t>2025-05-03T09:56:59.041921</t>
+  </si>
+  <si>
+    <t>2025-05-16T09:56:59.041928</t>
+  </si>
+  <si>
+    <t>2025-05-12T09:56:59.041936</t>
+  </si>
+  <si>
+    <t>2025-05-13T09:56:59.041950</t>
+  </si>
+  <si>
+    <t>2025-04-18T09:56:59.041957</t>
+  </si>
+  <si>
+    <t>2025-04-18T09:56:59.041964</t>
+  </si>
+  <si>
+    <t>2025-04-22T09:56:59.041971</t>
+  </si>
+  <si>
+    <t>2025-04-24T09:56:59.041978</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:56:59.041985</t>
+  </si>
+  <si>
+    <t>2025-05-16T09:56:59.041992</t>
+  </si>
+  <si>
+    <t>2025-04-22T09:56:59.041999</t>
+  </si>
+  <si>
+    <t>2025-05-12T09:56:59.042006</t>
+  </si>
+  <si>
+    <t>2025-05-01T09:56:59.042012</t>
+  </si>
+  <si>
+    <t>2025-04-25T09:56:59.042019</t>
+  </si>
+  <si>
+    <t>2025-05-10T09:56:59.042026</t>
+  </si>
+  <si>
+    <t>2025-04-26T09:56:59.042033</t>
+  </si>
+  <si>
+    <t>2024-08-01T10:00:00</t>
+  </si>
+  <si>
+    <t>2024-08-02T11:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -835,8 +925,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -869,11 +966,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -989,10 +1081,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="700">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1019,7 +1112,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1036,692 +1128,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{EC2D35FD-842D-4170-B25A-52A9DB32573C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1869,6 +1286,34 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1902,6 +1347,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-370F-413B-BB5C-A7AF2540E68A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1917,6 +1367,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-370F-413B-BB5C-A7AF2540E68A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2662,10 +2117,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Anik Sinhababu" refreshedDate="45755.672400115742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="40" xr:uid="{B98CDB42-F785-4AEA-9639-ED97E993FE81}">
   <cacheSource type="worksheet">
@@ -3030,7 +2481,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50ABE3CE-8E14-4C9E-B1B7-FEA7B34A5471}" name="PivotTable1" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50ABE3CE-8E14-4C9E-B1B7-FEA7B34A5471}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="C4:D7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -3074,11 +2525,35 @@
   <dataFields count="1">
     <dataField name="Count of Delete Status" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -3392,16 +2867,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.453125"/>
-    <col min="3" max="3" customWidth="true" width="15.6328125"/>
-    <col min="4" max="4" customWidth="true" width="11.7265625"/>
-    <col min="5" max="5" customWidth="true" width="28.6328125"/>
-    <col min="6" max="6" customWidth="true" width="21.54296875"/>
-    <col min="7" max="7" customWidth="true" width="18.90625"/>
-    <col min="8" max="8" customWidth="true" width="10.36328125"/>
-    <col min="9" max="9" customWidth="true" width="12.08984375"/>
-    <col min="10" max="10" customWidth="true" width="13.1796875"/>
-    <col min="11" max="11" customWidth="true" width="11.81640625"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3428,22 +2903,22 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>104</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -3451,22 +2926,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -3474,22 +2949,22 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>69</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>106</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -3497,22 +2972,22 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>70</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>107</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -3520,22 +2995,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>71</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>108</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -3543,22 +3018,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>72</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>109</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -3566,22 +3041,22 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>73</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>110</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -3589,22 +3064,22 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>74</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>111</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -3612,22 +3087,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>75</v>
       </c>
-      <c r="F10" t="s" s="0">
+      <c r="F10" t="s">
         <v>112</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -3635,22 +3110,22 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>75</v>
       </c>
-      <c r="F11" t="s" s="0">
+      <c r="F11" t="s">
         <v>113</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -3658,22 +3133,22 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>62</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" t="s" s="0">
+      <c r="F12" t="s">
         <v>114</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -3681,22 +3156,22 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>77</v>
       </c>
-      <c r="F13" t="s" s="0">
+      <c r="F13" t="s">
         <v>115</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3704,22 +3179,22 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="0">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>51</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>78</v>
       </c>
-      <c r="F14" t="s" s="0">
+      <c r="F14" t="s">
         <v>116</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3727,22 +3202,22 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="0">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>79</v>
       </c>
-      <c r="F15" t="s" s="0">
+      <c r="F15" t="s">
         <v>117</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3750,22 +3225,22 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="0">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>75</v>
       </c>
-      <c r="F16" t="s" s="0">
+      <c r="F16" t="s">
         <v>118</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -3773,22 +3248,22 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="0">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>80</v>
       </c>
-      <c r="F17" t="s" s="0">
+      <c r="F17" t="s">
         <v>119</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -3796,22 +3271,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="0">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>47</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>81</v>
       </c>
-      <c r="F18" t="s" s="0">
+      <c r="F18" t="s">
         <v>120</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -3819,22 +3294,22 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="0">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>62</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>82</v>
       </c>
-      <c r="F19" t="s" s="0">
+      <c r="F19" t="s">
         <v>121</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -3842,22 +3317,22 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="0">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>83</v>
       </c>
-      <c r="F20" t="s" s="0">
+      <c r="F20" t="s">
         <v>122</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -3865,22 +3340,22 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="0">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>84</v>
       </c>
-      <c r="F21" t="s" s="0">
+      <c r="F21" t="s">
         <v>123</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -3888,22 +3363,22 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="0">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>60</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>85</v>
       </c>
-      <c r="F22" t="s" s="0">
+      <c r="F22" t="s">
         <v>124</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -3911,22 +3386,22 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="0">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>86</v>
       </c>
-      <c r="F23" t="s" s="0">
+      <c r="F23" t="s">
         <v>125</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -3934,22 +3409,22 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="0">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="0">
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>87</v>
       </c>
-      <c r="F24" t="s" s="0">
+      <c r="F24" t="s">
         <v>126</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -3957,22 +3432,22 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="0">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>54</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>66</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>88</v>
       </c>
-      <c r="F25" t="s" s="0">
+      <c r="F25" t="s">
         <v>127</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -3980,22 +3455,22 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="0">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s" s="0">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" t="s" s="0">
+      <c r="D26" t="s">
         <v>65</v>
       </c>
-      <c r="E26" t="s" s="0">
+      <c r="E26" t="s">
         <v>89</v>
       </c>
-      <c r="F26" t="s" s="0">
+      <c r="F26" t="s">
         <v>128</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -4003,22 +3478,22 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="0">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s" s="0">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s" s="0">
+      <c r="C27" t="s">
         <v>49</v>
       </c>
-      <c r="D27" t="s" s="0">
+      <c r="D27" t="s">
         <v>61</v>
       </c>
-      <c r="E27" t="s" s="0">
+      <c r="E27" t="s">
         <v>90</v>
       </c>
-      <c r="F27" t="s" s="0">
+      <c r="F27" t="s">
         <v>129</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -4026,22 +3501,22 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="0">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s" s="0">
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s" s="0">
+      <c r="C28" t="s">
         <v>55</v>
       </c>
-      <c r="D28" t="s" s="0">
+      <c r="D28" t="s">
         <v>58</v>
       </c>
-      <c r="E28" t="s" s="0">
+      <c r="E28" t="s">
         <v>91</v>
       </c>
-      <c r="F28" t="s" s="0">
+      <c r="F28" t="s">
         <v>130</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -4049,22 +3524,22 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="0">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s" s="0">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" t="s" s="0">
+      <c r="C29" t="s">
         <v>48</v>
       </c>
-      <c r="D29" t="s" s="0">
+      <c r="D29" t="s">
         <v>66</v>
       </c>
-      <c r="E29" t="s" s="0">
+      <c r="E29" t="s">
         <v>92</v>
       </c>
-      <c r="F29" t="s" s="0">
+      <c r="F29" t="s">
         <v>131</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -4072,22 +3547,22 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="0">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s" s="0">
+      <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" t="s" s="0">
+      <c r="C30" t="s">
         <v>45</v>
       </c>
-      <c r="D30" t="s" s="0">
+      <c r="D30" t="s">
         <v>64</v>
       </c>
-      <c r="E30" t="s" s="0">
+      <c r="E30" t="s">
         <v>93</v>
       </c>
-      <c r="F30" t="s" s="0">
+      <c r="F30" t="s">
         <v>132</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -4095,22 +3570,22 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="0">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s" s="0">
+      <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="s" s="0">
+      <c r="C31" t="s">
         <v>53</v>
       </c>
-      <c r="D31" t="s" s="0">
+      <c r="D31" t="s">
         <v>66</v>
       </c>
-      <c r="E31" t="s" s="0">
+      <c r="E31" t="s">
         <v>94</v>
       </c>
-      <c r="F31" t="s" s="0">
+      <c r="F31" t="s">
         <v>133</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -4118,22 +3593,22 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="0">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s" s="0">
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" t="s" s="0">
+      <c r="C32" t="s">
         <v>44</v>
       </c>
-      <c r="D32" t="s" s="0">
+      <c r="D32" t="s">
         <v>64</v>
       </c>
-      <c r="E32" t="s" s="0">
+      <c r="E32" t="s">
         <v>95</v>
       </c>
-      <c r="F32" t="s" s="0">
+      <c r="F32" t="s">
         <v>134</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -4141,22 +3616,22 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="0">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s" s="0">
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33" t="s" s="0">
+      <c r="C33" t="s">
         <v>46</v>
       </c>
-      <c r="D33" t="s" s="0">
+      <c r="D33" t="s">
         <v>61</v>
       </c>
-      <c r="E33" t="s" s="0">
+      <c r="E33" t="s">
         <v>96</v>
       </c>
-      <c r="F33" t="s" s="0">
+      <c r="F33" t="s">
         <v>135</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -4164,22 +3639,22 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="0">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s" s="0">
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" t="s" s="0">
+      <c r="C34" t="s">
         <v>56</v>
       </c>
-      <c r="D34" t="s" s="0">
+      <c r="D34" t="s">
         <v>62</v>
       </c>
-      <c r="E34" t="s" s="0">
+      <c r="E34" t="s">
         <v>97</v>
       </c>
-      <c r="F34" t="s" s="0">
+      <c r="F34" t="s">
         <v>136</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -4187,22 +3662,22 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="0">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s" s="0">
+      <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35" t="s" s="0">
+      <c r="C35" t="s">
         <v>49</v>
       </c>
-      <c r="D35" t="s" s="0">
+      <c r="D35" t="s">
         <v>57</v>
       </c>
-      <c r="E35" t="s" s="0">
+      <c r="E35" t="s">
         <v>98</v>
       </c>
-      <c r="F35" t="s" s="0">
+      <c r="F35" t="s">
         <v>137</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -4210,22 +3685,22 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="0">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s" s="0">
+      <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" t="s" s="0">
+      <c r="C36" t="s">
         <v>56</v>
       </c>
-      <c r="D36" t="s" s="0">
+      <c r="D36" t="s">
         <v>63</v>
       </c>
-      <c r="E36" t="s" s="0">
+      <c r="E36" t="s">
         <v>99</v>
       </c>
-      <c r="F36" t="s" s="0">
+      <c r="F36" t="s">
         <v>138</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -4233,22 +3708,22 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="0">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s" s="0">
+      <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s" s="0">
+      <c r="C37" t="s">
         <v>55</v>
       </c>
-      <c r="D37" t="s" s="0">
+      <c r="D37" t="s">
         <v>66</v>
       </c>
-      <c r="E37" t="s" s="0">
+      <c r="E37" t="s">
         <v>100</v>
       </c>
-      <c r="F37" t="s" s="0">
+      <c r="F37" t="s">
         <v>139</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -4256,22 +3731,22 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="0">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s" s="0">
+      <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" t="s" s="0">
+      <c r="C38" t="s">
         <v>48</v>
       </c>
-      <c r="D38" t="s" s="0">
+      <c r="D38" t="s">
         <v>64</v>
       </c>
-      <c r="E38" t="s" s="0">
+      <c r="E38" t="s">
         <v>101</v>
       </c>
-      <c r="F38" t="s" s="0">
+      <c r="F38" t="s">
         <v>140</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -4279,22 +3754,22 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="0">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="s" s="0">
+      <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" t="s" s="0">
+      <c r="C39" t="s">
         <v>46</v>
       </c>
-      <c r="D39" t="s" s="0">
+      <c r="D39" t="s">
         <v>59</v>
       </c>
-      <c r="E39" t="s" s="0">
+      <c r="E39" t="s">
         <v>102</v>
       </c>
-      <c r="F39" t="s" s="0">
+      <c r="F39" t="s">
         <v>141</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -4302,22 +3777,22 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="0">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s" s="0">
+      <c r="B40" t="s">
         <v>38</v>
       </c>
-      <c r="C40" t="s" s="0">
+      <c r="C40" t="s">
         <v>49</v>
       </c>
-      <c r="D40" t="s" s="0">
+      <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s" s="0">
+      <c r="E40" t="s">
         <v>98</v>
       </c>
-      <c r="F40" t="s" s="0">
+      <c r="F40" t="s">
         <v>142</v>
       </c>
       <c r="G40" s="2" t="s">
@@ -4325,22 +3800,22 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="0">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="s" s="0">
+      <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="C41" t="s" s="0">
+      <c r="C41" t="s">
         <v>47</v>
       </c>
-      <c r="D41" t="s" s="0">
+      <c r="D41" t="s">
         <v>64</v>
       </c>
-      <c r="E41" t="s" s="0">
+      <c r="E41" t="s">
         <v>103</v>
       </c>
-      <c r="F41" t="s" s="0">
+      <c r="F41" t="s">
         <v>143</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -4365,12 +3840,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="19.08984375"/>
-    <col min="3" max="3" customWidth="true" width="13.36328125"/>
-    <col min="4" max="4" customWidth="true" width="12.1796875"/>
-    <col min="5" max="5" customWidth="true" width="25.1796875"/>
-    <col min="6" max="6" customWidth="true" width="15.0"/>
-    <col min="7" max="7" customWidth="true" width="17.6328125"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5331,27 +4806,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.1796875"/>
-    <col min="2" max="2" customWidth="true" width="22.54296875"/>
-    <col min="3" max="3" customWidth="true" width="20.6328125"/>
-    <col min="4" max="4" customWidth="true" width="17.81640625"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="28.0"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="15">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -5362,7 +4837,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -5373,7 +4848,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -5384,7 +4859,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -5395,7 +4870,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -5406,7 +4881,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -5417,7 +4892,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -5428,7 +4903,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -5439,7 +4914,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -5450,7 +4925,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -5470,713 +4945,713 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7258E2C3-1C99-4E05-9F85-35EF852783B3}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.90625"/>
-    <col min="2" max="2" customWidth="true" width="15.0"/>
-    <col min="3" max="3" customWidth="true" width="16.26953125"/>
-    <col min="4" max="4" customWidth="true" width="19.453125"/>
-    <col min="5" max="5" customWidth="true" width="15.08984375"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="580">
-        <v>229</v>
-      </c>
-      <c r="C2" t="s" s="660">
-        <v>229</v>
-      </c>
-      <c r="D2" t="s" s="540">
-        <v>229</v>
-      </c>
-      <c r="E2" t="s" s="620">
+      <c r="B2" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="581">
-        <v>229</v>
-      </c>
-      <c r="C3" t="s" s="661">
-        <v>229</v>
-      </c>
-      <c r="D3" t="s" s="541">
-        <v>229</v>
-      </c>
-      <c r="E3" t="s" s="621">
+      <c r="B3" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="582">
-        <v>229</v>
-      </c>
-      <c r="C4" t="s" s="662">
-        <v>229</v>
-      </c>
-      <c r="D4" t="s" s="542">
-        <v>229</v>
-      </c>
-      <c r="E4" t="s" s="622">
+      <c r="B4" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s" s="583">
+      <c r="B5" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C5" t="s" s="663">
-        <v>229</v>
-      </c>
-      <c r="D5" t="s" s="543">
-        <v>229</v>
-      </c>
-      <c r="E5" t="s" s="623">
+      <c r="C5" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s" s="584">
+      <c r="B6" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C6" t="s" s="664">
-        <v>229</v>
-      </c>
-      <c r="D6" t="s" s="544">
-        <v>229</v>
-      </c>
-      <c r="E6" t="s" s="624">
+      <c r="C6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="585">
-        <v>229</v>
-      </c>
-      <c r="C7" t="s" s="665">
-        <v>229</v>
-      </c>
-      <c r="D7" t="s" s="545">
-        <v>229</v>
-      </c>
-      <c r="E7" t="s" s="625">
+      <c r="B7" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s" s="586">
+      <c r="B8" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C8" t="s" s="666">
-        <v>229</v>
-      </c>
-      <c r="D8" t="s" s="546">
-        <v>229</v>
-      </c>
-      <c r="E8" t="s" s="626">
+      <c r="C8" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s" s="587">
+      <c r="B9" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C9" t="s" s="667">
-        <v>229</v>
-      </c>
-      <c r="D9" t="s" s="547">
-        <v>229</v>
-      </c>
-      <c r="E9" t="s" s="627">
+      <c r="C9" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s" s="588">
+      <c r="B10" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C10" t="s" s="668">
-        <v>229</v>
-      </c>
-      <c r="D10" t="s" s="548">
-        <v>229</v>
-      </c>
-      <c r="E10" t="s" s="628">
+      <c r="C10" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s" s="589">
+      <c r="B11" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C11" t="s" s="669">
-        <v>229</v>
-      </c>
-      <c r="D11" t="s" s="549">
-        <v>229</v>
-      </c>
-      <c r="E11" t="s" s="629">
+      <c r="C11" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s" s="590">
+      <c r="B12" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C12" t="s" s="670">
-        <v>229</v>
-      </c>
-      <c r="D12" t="s" s="550">
-        <v>229</v>
-      </c>
-      <c r="E12" t="s" s="630">
+      <c r="C12" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s" s="591">
+      <c r="B13" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C13" t="s" s="671">
-        <v>229</v>
-      </c>
-      <c r="D13" t="s" s="551">
-        <v>229</v>
-      </c>
-      <c r="E13" t="s" s="631">
+      <c r="C13" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s" s="592">
+      <c r="B14" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C14" t="s" s="672">
-        <v>229</v>
-      </c>
-      <c r="D14" t="s" s="552">
-        <v>229</v>
-      </c>
-      <c r="E14" t="s" s="632">
+      <c r="C14" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s" s="593">
+      <c r="B15" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C15" t="s" s="673">
-        <v>229</v>
-      </c>
-      <c r="D15" t="s" s="553">
-        <v>229</v>
-      </c>
-      <c r="E15" t="s" s="633">
+      <c r="C15" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="594">
+      <c r="B16" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C16" t="s" s="674">
-        <v>229</v>
-      </c>
-      <c r="D16" t="s" s="554">
-        <v>229</v>
-      </c>
-      <c r="E16" t="s" s="634">
+      <c r="C16" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s" s="595">
-        <v>229</v>
-      </c>
-      <c r="C17" t="s" s="675">
-        <v>229</v>
-      </c>
-      <c r="D17" t="s" s="555">
-        <v>229</v>
-      </c>
-      <c r="E17" t="s" s="635">
+      <c r="B17" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s" s="596">
+      <c r="B18" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C18" t="s" s="676">
-        <v>229</v>
-      </c>
-      <c r="D18" t="s" s="556">
-        <v>229</v>
-      </c>
-      <c r="E18" t="s" s="636">
+      <c r="C18" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s" s="597">
-        <v>229</v>
-      </c>
-      <c r="C19" t="s" s="677">
-        <v>229</v>
-      </c>
-      <c r="D19" t="s" s="557">
-        <v>229</v>
-      </c>
-      <c r="E19" t="s" s="637">
+      <c r="B19" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s" s="598">
+      <c r="B20" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C20" t="s" s="678">
-        <v>229</v>
-      </c>
-      <c r="D20" t="s" s="558">
-        <v>229</v>
-      </c>
-      <c r="E20" t="s" s="638">
+      <c r="C20" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s" s="599">
+      <c r="B21" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C21" t="s" s="679">
-        <v>229</v>
-      </c>
-      <c r="D21" t="s" s="559">
-        <v>229</v>
-      </c>
-      <c r="E21" t="s" s="639">
+      <c r="C21" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s" s="600">
+      <c r="B22" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C22" t="s" s="680">
-        <v>229</v>
-      </c>
-      <c r="D22" t="s" s="560">
-        <v>229</v>
-      </c>
-      <c r="E22" t="s" s="640">
+      <c r="C22" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s" s="601">
-        <v>229</v>
-      </c>
-      <c r="C23" t="s" s="681">
-        <v>229</v>
-      </c>
-      <c r="D23" t="s" s="561">
-        <v>229</v>
-      </c>
-      <c r="E23" t="s" s="641">
+      <c r="B23" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s" s="602">
-        <v>229</v>
-      </c>
-      <c r="C24" t="s" s="682">
-        <v>229</v>
-      </c>
-      <c r="D24" t="s" s="562">
-        <v>229</v>
-      </c>
-      <c r="E24" t="s" s="642">
+      <c r="B24" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s" s="603">
+      <c r="B25" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C25" t="s" s="683">
-        <v>229</v>
-      </c>
-      <c r="D25" t="s" s="563">
-        <v>229</v>
-      </c>
-      <c r="E25" t="s" s="643">
+      <c r="C25" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s" s="604">
+      <c r="B26" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C26" t="s" s="684">
-        <v>229</v>
-      </c>
-      <c r="D26" t="s" s="564">
-        <v>229</v>
-      </c>
-      <c r="E26" t="s" s="644">
+      <c r="C26" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s" s="605">
+      <c r="B27" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C27" t="s" s="685">
-        <v>229</v>
-      </c>
-      <c r="D27" t="s" s="565">
-        <v>229</v>
-      </c>
-      <c r="E27" t="s" s="645">
+      <c r="C27" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B28" t="s" s="606">
-        <v>229</v>
-      </c>
-      <c r="C28" t="s" s="686">
-        <v>229</v>
-      </c>
-      <c r="D28" t="s" s="566">
-        <v>229</v>
-      </c>
-      <c r="E28" t="s" s="646">
+      <c r="B28" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B29" t="s" s="607">
-        <v>229</v>
-      </c>
-      <c r="C29" t="s" s="687">
-        <v>229</v>
-      </c>
-      <c r="D29" t="s" s="567">
-        <v>229</v>
-      </c>
-      <c r="E29" t="s" s="647">
+      <c r="B29" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B30" t="s" s="608">
-        <v>229</v>
-      </c>
-      <c r="C30" t="s" s="688">
-        <v>229</v>
-      </c>
-      <c r="D30" t="s" s="568">
-        <v>229</v>
-      </c>
-      <c r="E30" t="s" s="648">
+      <c r="B30" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B31" t="s" s="609">
+      <c r="B31" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C31" t="s" s="689">
-        <v>229</v>
-      </c>
-      <c r="D31" t="s" s="569">
-        <v>229</v>
-      </c>
-      <c r="E31" t="s" s="649">
+      <c r="C31" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s" s="610">
-        <v>229</v>
-      </c>
-      <c r="C32" t="s" s="690">
-        <v>229</v>
-      </c>
-      <c r="D32" t="s" s="570">
-        <v>229</v>
-      </c>
-      <c r="E32" t="s" s="650">
+      <c r="B32" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B33" t="s" s="611">
-        <v>229</v>
-      </c>
-      <c r="C33" t="s" s="691">
-        <v>229</v>
-      </c>
-      <c r="D33" t="s" s="571">
-        <v>229</v>
-      </c>
-      <c r="E33" t="s" s="651">
+      <c r="B33" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B34" t="s" s="612">
+      <c r="B34" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C34" t="s" s="692">
-        <v>229</v>
-      </c>
-      <c r="D34" t="s" s="572">
-        <v>229</v>
-      </c>
-      <c r="E34" t="s" s="652">
+      <c r="C34" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B35" t="s" s="613">
-        <v>229</v>
-      </c>
-      <c r="C35" t="s" s="693">
-        <v>229</v>
-      </c>
-      <c r="D35" t="s" s="573">
-        <v>229</v>
-      </c>
-      <c r="E35" t="s" s="653">
+      <c r="B35" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E35" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B36" t="s" s="614">
-        <v>229</v>
-      </c>
-      <c r="C36" t="s" s="694">
-        <v>229</v>
-      </c>
-      <c r="D36" t="s" s="574">
-        <v>229</v>
-      </c>
-      <c r="E36" t="s" s="654">
+      <c r="B36" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E36" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B37" t="s" s="615">
-        <v>229</v>
-      </c>
-      <c r="C37" t="s" s="695">
-        <v>229</v>
-      </c>
-      <c r="D37" t="s" s="575">
-        <v>229</v>
-      </c>
-      <c r="E37" t="s" s="655">
+      <c r="B37" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B38" t="s" s="616">
+      <c r="B38" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C38" t="s" s="696">
-        <v>229</v>
-      </c>
-      <c r="D38" t="s" s="576">
-        <v>229</v>
-      </c>
-      <c r="E38" t="s" s="656">
+      <c r="C38" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B39" t="s" s="617">
-        <v>229</v>
-      </c>
-      <c r="C39" t="s" s="697">
-        <v>229</v>
-      </c>
-      <c r="D39" t="s" s="577">
-        <v>229</v>
-      </c>
-      <c r="E39" t="s" s="657">
+      <c r="B39" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s" s="618">
+      <c r="B40" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C40" t="s" s="698">
-        <v>229</v>
-      </c>
-      <c r="D40" t="s" s="578">
-        <v>229</v>
-      </c>
-      <c r="E40" t="s" s="658">
+      <c r="C40" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B41" t="s" s="619">
+      <c r="B41" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C41" t="s" s="699">
-        <v>229</v>
-      </c>
-      <c r="D41" t="s" s="579">
-        <v>229</v>
-      </c>
-      <c r="E41" t="s" s="659">
+      <c r="C41" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" s="17" t="s">
         <v>230</v>
       </c>
     </row>
@@ -6195,45 +5670,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="3.6328125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.26953125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.90625"/>
+    <col min="2" max="2" width="3.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C5" t="s" s="0">
-        <v>229</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="C5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>256</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7">
         <v>40</v>
       </c>
     </row>
@@ -6241,4 +5716,485 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95EB6068-4D8E-4E4B-A7E2-929A05DE72A4}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19">
+        <v>2861</v>
+      </c>
+      <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19">
+        <v>9981</v>
+      </c>
+      <c r="C3" s="19">
+        <v>8</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
+        <v>8028</v>
+      </c>
+      <c r="C4" s="19">
+        <v>3</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1036</v>
+      </c>
+      <c r="C5" s="19">
+        <v>7</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F5" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19">
+        <v>9322</v>
+      </c>
+      <c r="C6" s="19">
+        <v>8</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F6" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19">
+        <v>5843</v>
+      </c>
+      <c r="C7" s="19">
+        <v>4</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19">
+        <v>3552</v>
+      </c>
+      <c r="C8" s="19">
+        <v>6</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F8" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="19">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19">
+        <v>8245</v>
+      </c>
+      <c r="C9" s="19">
+        <v>3</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="19">
+        <v>3767</v>
+      </c>
+      <c r="C10" s="19">
+        <v>2</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19">
+        <v>6107</v>
+      </c>
+      <c r="C11" s="19">
+        <v>4</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F11" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19">
+        <v>8052</v>
+      </c>
+      <c r="C12" s="19">
+        <v>4</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19">
+        <v>5761</v>
+      </c>
+      <c r="C13" s="19">
+        <v>2</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19">
+        <v>8973</v>
+      </c>
+      <c r="C14" s="19">
+        <v>3</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="19">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19">
+        <v>4924</v>
+      </c>
+      <c r="C15" s="19">
+        <v>3</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F15" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="19">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19">
+        <v>1125</v>
+      </c>
+      <c r="C16" s="19">
+        <v>2</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F16" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="19">
+        <v>16</v>
+      </c>
+      <c r="B17" s="19">
+        <v>2933</v>
+      </c>
+      <c r="C17" s="19">
+        <v>9</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="F17" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="19">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19">
+        <v>9745</v>
+      </c>
+      <c r="C18" s="19">
+        <v>10</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="F18" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19">
+        <v>3860</v>
+      </c>
+      <c r="C19" s="19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F19" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="19">
+        <v>19</v>
+      </c>
+      <c r="B20" s="19">
+        <v>4425</v>
+      </c>
+      <c r="C20" s="19">
+        <v>10</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="19">
+        <v>20</v>
+      </c>
+      <c r="B21" s="19">
+        <v>2957</v>
+      </c>
+      <c r="C21" s="19">
+        <v>7</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F21" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="19">
+        <v>21</v>
+      </c>
+      <c r="B22" s="19">
+        <v>1234</v>
+      </c>
+      <c r="C22" s="19">
+        <v>5</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="F22" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="19">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19">
+        <v>5678</v>
+      </c>
+      <c r="C23" s="19">
+        <v>3</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F23" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>